<commit_message>
seperate actions into two files
</commit_message>
<xml_diff>
--- a/L2_cousework/car_complaint.xlsx
+++ b/L2_cousework/car_complaint.xlsx
@@ -933,7 +933,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>信息审核</t>
+          <t>厂家受理</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>信息审核</t>
+          <t>厂家受理</t>
         </is>
       </c>
     </row>

</xml_diff>